<commit_message>
Dependent dropdown second implementation
</commit_message>
<xml_diff>
--- a/DropFtr.xlsx
+++ b/DropFtr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudipRana\Desktop\POI-Practise\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6A42D0-2322-4530-8840-CF9F425A1D3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66736AD5-8A34-4181-9D6E-81A636C40564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>CHOICES</t>
   </si>
@@ -49,6 +49,27 @@
   </si>
   <si>
     <t>NO_CHOICES</t>
+  </si>
+  <si>
+    <t>INC</t>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>DEF</t>
   </si>
 </sst>
 </file>
@@ -366,44 +387,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D1:E5"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Contains VBA-Macro code along with other POCs
</commit_message>
<xml_diff>
--- a/DropFtr.xlsx
+++ b/DropFtr.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SudipRana\Desktop\POI-Practise\poi\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66736AD5-8A34-4181-9D6E-81A636C40564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6708889A-7139-4E26-A00E-A5CF1282FFA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="29070" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>CHOICES</t>
   </si>
@@ -64,12 +60,6 @@
   </si>
   <si>
     <t>Completed</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>DEF</t>
   </si>
 </sst>
 </file>
@@ -390,7 +380,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,9 +405,6 @@
       <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
@@ -435,9 +422,6 @@
       <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
@@ -467,16 +451,10 @@
       <c r="A9">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>